<commit_message>
select database with color
</commit_message>
<xml_diff>
--- a/Update.xlsx
+++ b/Update.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AFIF TEC\Desktop\git_project\AlHall\Update_AlHal\www\www\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20388" windowHeight="8376"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -19,7 +24,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -109,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -170,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="C8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0">
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -230,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0">
+    <comment ref="C10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -260,7 +265,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0">
+    <comment ref="C11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -291,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0">
+    <comment ref="C12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -326,7 +331,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Messions</t>
   </si>
@@ -490,19 +495,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -510,7 +511,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -518,163 +519,23 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -705,194 +566,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -900,264 +575,22 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1178,57 +611,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1240,6 +628,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1524,30 +920,30 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="35.5714285714286" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.14285714285714" style="3"/>
-    <col min="3" max="3" width="48.5714285714286" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.8571428571429" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.14285714285714" style="3"/>
-    <col min="7" max="7" width="19.8571428571429" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="9.14285714285714" style="3"/>
+    <col min="1" max="1" width="35.59765625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.09765625" style="3"/>
+    <col min="3" max="3" width="48.59765625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.8984375" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.09765625" style="3"/>
+    <col min="7" max="7" width="19.8984375" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.09765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="21" spans="1:4">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="21">
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="1" t="s">
@@ -1558,7 +954,7 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="2">
+      <c r="A2" s="11">
         <f>DATE(2021,12,14)</f>
         <v>44544</v>
       </c>
@@ -1583,7 +979,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="1:11">
+      <c r="A3" s="11"/>
       <c r="B3" s="8">
         <f t="shared" ref="B3:B42" si="0">ROW()-1</f>
         <v>2</v>
@@ -1602,7 +999,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="1:11">
+      <c r="A4" s="11"/>
       <c r="B4" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1618,7 +1016,8 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="1:11">
+      <c r="A5" s="11"/>
       <c r="B5" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1631,7 +1030,8 @@
       </c>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="1:11">
+      <c r="A6" s="11"/>
       <c r="B6" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1644,7 +1044,8 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="1:11">
+      <c r="A7" s="11"/>
       <c r="B7" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1659,7 +1060,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="1:11">
+      <c r="A8" s="11"/>
       <c r="B8" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1671,7 +1073,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="1:11">
+      <c r="A9" s="11"/>
       <c r="B9" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1683,7 +1086,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="1:11">
+      <c r="A10" s="11"/>
       <c r="B10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1695,7 +1099,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="1:11">
+      <c r="A11" s="11"/>
       <c r="B11" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1707,7 +1112,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="1:11">
+      <c r="A12" s="11"/>
       <c r="B12" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1719,8 +1125,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2">
+    <row r="13" spans="1:11">
+      <c r="A13" s="11">
         <f>DATE(2021,12,15)</f>
         <v>44545</v>
       </c>
@@ -1732,7 +1138,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="1:11">
+      <c r="A14" s="11"/>
       <c r="B14" s="10">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1741,7 +1148,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="1:11">
+      <c r="A15" s="11"/>
       <c r="B15" s="10">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1750,7 +1158,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="1:11">
+      <c r="A16" s="11"/>
       <c r="B16" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1759,7 +1168,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="1:4">
+      <c r="A17" s="11"/>
       <c r="B17" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1768,7 +1178,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="1:4">
+      <c r="A18" s="11"/>
       <c r="B18" s="10">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1777,7 +1188,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="1:4">
+      <c r="A19" s="11"/>
       <c r="B19" s="10">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1786,7 +1198,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="1:4">
+      <c r="A20" s="11"/>
       <c r="B20" s="10">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1795,17 +1208,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="10">
+    <row r="21" spans="1:4">
+      <c r="A21" s="11"/>
+      <c r="B21" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="2">
+      <c r="D21" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="11">
         <f>DATE(2021,12,16)</f>
         <v>44546</v>
       </c>
@@ -1817,7 +1234,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="1:4">
+      <c r="A23" s="11"/>
       <c r="B23" s="10">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1826,7 +1244,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="1:4">
+      <c r="A24" s="11"/>
       <c r="B24" s="10">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1835,7 +1254,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="1:4">
+      <c r="A25" s="11"/>
       <c r="B25" s="10">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1844,7 +1264,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="1:4">
+      <c r="A26" s="11"/>
       <c r="B26" s="10">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1853,7 +1274,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="1:4">
+      <c r="A27" s="11"/>
       <c r="B27" s="10">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1862,7 +1284,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="1:4">
+      <c r="A28" s="11"/>
       <c r="B28" s="10">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1871,7 +1294,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="1:4">
+      <c r="A29" s="11"/>
       <c r="B29" s="10">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1880,7 +1304,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="1:4">
+      <c r="A30" s="11"/>
       <c r="B30" s="10">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1889,8 +1314,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="2">
+    <row r="31" spans="1:4">
+      <c r="A31" s="11">
         <f>DATE(2021,12,18)</f>
         <v>44548</v>
       </c>
@@ -1902,7 +1327,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="1:4">
+      <c r="A32" s="11"/>
       <c r="B32" s="10">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1911,7 +1337,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="1:3">
+      <c r="A33" s="11"/>
       <c r="B33" s="10">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1920,7 +1347,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="1:3">
+      <c r="A34" s="11"/>
       <c r="B34" s="10">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1929,7 +1357,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="1:3">
+      <c r="A35" s="11"/>
       <c r="B35" s="10">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1938,7 +1367,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="1:3">
+      <c r="A36" s="11"/>
       <c r="B36" s="10">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1947,7 +1377,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="1:3">
+      <c r="A37" s="11"/>
       <c r="B37" s="10">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1956,7 +1387,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="1:3">
+      <c r="A38" s="11"/>
       <c r="B38" s="10">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1965,25 +1397,25 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="2:2">
+    <row r="39" spans="1:3">
       <c r="B39" s="10">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="2:2">
+    <row r="40" spans="1:3">
       <c r="B40" s="10">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="2:2">
+    <row r="41" spans="1:3">
       <c r="B41" s="10">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="2:2">
+    <row r="42" spans="1:3">
       <c r="B42" s="10">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1996,12 +1428,12 @@
     <mergeCell ref="A22:A30"/>
     <mergeCell ref="A31:A38"/>
   </mergeCells>
-  <conditionalFormatting sqref="A:D">
+  <conditionalFormatting sqref="A1:D1048576">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A:C">
+  <conditionalFormatting sqref="A1:C1048576">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
@@ -2011,9 +1443,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>